<commit_message>
Added reading for 1/27
</commit_message>
<xml_diff>
--- a/CSC530_reading_schedule_Wi2017.xlsx
+++ b/CSC530_reading_schedule_Wi2017.xlsx
@@ -165,10 +165,6 @@
   </si>
   <si>
     <t xml:space="preserve">- Think Python, Chp 2-3, 5
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Think Python, Chp 6-7
 </t>
   </si>
   <si>
@@ -264,6 +260,34 @@
   </si>
   <si>
     <t xml:space="preserve">Short Assignments </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Think Python, Chp 6-7
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Stan Ulam, John Von Neumann, and the Monte Carlo Method," </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Eckhardt
+</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -842,7 +866,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,7 +882,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -911,7 +935,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>4</v>
@@ -1029,7 +1053,7 @@
       </c>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="8">
         <v>42396</v>
@@ -1037,7 +1061,7 @@
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="17" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
@@ -1057,7 +1081,7 @@
         <v>10</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F18" s="7"/>
     </row>
@@ -1069,7 +1093,7 @@
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
@@ -1089,11 +1113,11 @@
         <v>11</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1104,7 +1128,7 @@
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
@@ -1118,13 +1142,13 @@
         <v>42415</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>12</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G24" s="7"/>
     </row>
@@ -1147,11 +1171,11 @@
         <v>42422</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F27" s="10" t="s">
         <v>13</v>
@@ -1166,7 +1190,7 @@
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
@@ -1205,11 +1229,11 @@
         <v>42437</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="10" t="s">
@@ -1239,7 +1263,7 @@
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
@@ -1267,7 +1291,7 @@
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
@@ -1291,7 +1315,7 @@
         <v>42458</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>

</xml_diff>